<commit_message>
fmcw_demo: fix input capture, add dac init and update pinout
</commit_message>
<xml_diff>
--- a/embeded/fmcw_demo/DOC/pin分配.xlsx
+++ b/embeded/fmcw_demo/DOC/pin分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,10 +251,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PC5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DIVOUT_MCU</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -464,6 +460,26 @@
   </si>
   <si>
     <t>SPI4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIM1_CH1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAC_OUT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC123_IN0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC123_IN1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -488,12 +504,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -562,7 +584,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -578,10 +600,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -886,7 +911,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -896,7 +921,8 @@
     <col min="4" max="4" width="29.19921875" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.06640625" style="2"/>
     <col min="6" max="6" width="24.53125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="2"/>
+    <col min="7" max="7" width="11.1328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -919,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -937,9 +963,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
@@ -955,8 +983,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
@@ -972,43 +1002,47 @@
         <v>28</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1016,18 +1050,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1035,18 +1069,18 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1054,18 +1088,18 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1076,14 +1110,14 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1095,13 +1129,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
@@ -1112,13 +1146,13 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
@@ -1129,13 +1163,13 @@
         <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
@@ -1146,13 +1180,13 @@
         <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7">
@@ -1163,13 +1197,13 @@
         <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
@@ -1180,13 +1214,13 @@
         <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
@@ -1197,13 +1231,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
@@ -1214,13 +1248,13 @@
         <v>54</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7">
@@ -1231,13 +1265,13 @@
         <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
@@ -1248,13 +1282,13 @@
         <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7">
@@ -1265,13 +1299,13 @@
         <v>29</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7">
@@ -1282,13 +1316,13 @@
         <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
@@ -1299,13 +1333,13 @@
         <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="6"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7">
@@ -1323,10 +1357,10 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1343,8 +1377,8 @@
         <v>40</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1">
@@ -1354,17 +1388,17 @@
         <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1374,14 +1408,14 @@
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="6"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1399,7 +1433,7 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1417,7 +1451,7 @@
         <v>47</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="6"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7">
@@ -1435,10 +1469,10 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1446,67 +1480,67 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="5"/>
+      <c r="F34" s="6"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7">
@@ -1514,16 +1548,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="5"/>
+      <c r="F35" s="6"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7">
@@ -1531,16 +1565,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="6"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7">
@@ -1548,16 +1582,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="5"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7">
@@ -1565,16 +1599,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="5"/>
+      <c r="F38" s="6"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7">
@@ -1582,16 +1616,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E39" s="1"/>
-      <c r="F39" s="5"/>
+      <c r="F39" s="6"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7">
@@ -1599,16 +1633,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="5"/>
+      <c r="F40" s="6"/>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7">
@@ -1616,16 +1650,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="5"/>
+      <c r="F41" s="6"/>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7">
@@ -1633,16 +1667,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="5"/>
+      <c r="F42" s="6"/>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7">
@@ -1650,16 +1684,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E43" s="1"/>
-      <c r="F43" s="5"/>
+      <c r="F43" s="6"/>
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7">
@@ -1667,16 +1701,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E44" s="1"/>
-      <c r="F44" s="5"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7">
@@ -1684,16 +1718,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="6"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fmcw_demo: big improvment list below
1. update pinout;
2. add final demo board sch pcb;
3. add fpga gpio init;
4. add led output;
5. add usb gpio init(reset);
6. update adc.c;
7. add uart1 test;
8. update usb bsp;
9. add mem entry;
10. add algo entry;
</commit_message>
<xml_diff>
--- a/embeded/fmcw_demo/DOC/pin分配.xlsx
+++ b/embeded/fmcw_demo/DOC/pin分配.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="STM32F429" sheetId="1" r:id="rId1"/>
+    <sheet name="STM32F429VE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -480,6 +480,110 @@
   </si>
   <si>
     <t>ADC123_IN1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PE14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_T2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_T3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -504,18 +608,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -584,7 +682,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -600,13 +698,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -908,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -961,7 +1056,9 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F2" s="4" t="s">
         <v>95</v>
       </c>
@@ -982,8 +1079,10 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
         <v>122</v>
       </c>
@@ -1002,7 +1101,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="1" t="s">
         <v>120</v>
       </c>
@@ -1011,7 +1110,7 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1021,7 +1120,7 @@
         <v>60</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="1" t="s">
         <v>119</v>
       </c>
@@ -1040,7 +1139,7 @@
         <v>68</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="1" t="s">
         <v>116</v>
       </c>
@@ -1059,7 +1158,7 @@
         <v>69</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="1" t="s">
         <v>117</v>
       </c>
@@ -1077,8 +1176,10 @@
       <c r="D8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="1" t="s">
         <v>100</v>
       </c>
@@ -1097,7 +1198,7 @@
         <v>71</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1" t="s">
         <v>117</v>
       </c>
@@ -1119,7 +1220,9 @@
       <c r="F10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
@@ -1135,8 +1238,10 @@
         <v>12</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
@@ -1152,8 +1257,10 @@
         <v>13</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
@@ -1169,8 +1276,10 @@
         <v>16</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1">
@@ -1186,8 +1295,10 @@
         <v>17</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1">
@@ -1203,8 +1314,10 @@
         <v>18</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1">
@@ -1220,8 +1333,10 @@
         <v>19</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1">
@@ -1237,8 +1352,10 @@
         <v>20</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1">
@@ -1254,8 +1371,10 @@
         <v>55</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1">
@@ -1271,8 +1390,10 @@
         <v>57</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1">
@@ -1288,8 +1409,10 @@
         <v>59</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="1"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1">
@@ -1305,8 +1428,10 @@
         <v>30</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="1"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1">
@@ -1322,7 +1447,7 @@
         <v>34</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
@@ -1339,7 +1464,7 @@
         <v>32</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7">
@@ -1377,8 +1502,8 @@
         <v>40</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1">
@@ -1408,12 +1533,12 @@
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="1" t="s">
         <v>101</v>
       </c>
@@ -1451,7 +1576,7 @@
         <v>47</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="6"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7">
@@ -1489,8 +1614,8 @@
         <v>64</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1">
@@ -1506,8 +1631,8 @@
         <v>65</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1">
@@ -1523,8 +1648,8 @@
         <v>66</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1">
@@ -1540,7 +1665,7 @@
         <v>76</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="6"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7">
@@ -1557,7 +1682,7 @@
         <v>77</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="6"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7">
@@ -1574,7 +1699,7 @@
         <v>78</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="6"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7">
@@ -1591,7 +1716,7 @@
         <v>79</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="6"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7">
@@ -1608,7 +1733,7 @@
         <v>80</v>
       </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="6"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7">
@@ -1625,7 +1750,7 @@
         <v>81</v>
       </c>
       <c r="E39" s="1"/>
-      <c r="F39" s="6"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7">
@@ -1642,7 +1767,7 @@
         <v>82</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="6"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7">
@@ -1659,7 +1784,7 @@
         <v>83</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="6"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7">
@@ -1676,7 +1801,7 @@
         <v>84</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="6"/>
+      <c r="F42" s="5"/>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7">
@@ -1693,7 +1818,7 @@
         <v>85</v>
       </c>
       <c r="E43" s="1"/>
-      <c r="F43" s="6"/>
+      <c r="F43" s="5"/>
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7">
@@ -1710,7 +1835,7 @@
         <v>86</v>
       </c>
       <c r="E44" s="1"/>
-      <c r="F44" s="6"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7">
@@ -1730,17 +1855,105 @@
       <c r="F45" s="5"/>
       <c r="G45" s="1"/>
     </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="F48:F50"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="G30:G33"/>
-    <mergeCell ref="F30:F45"/>
     <mergeCell ref="F2:F9"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="F10:F23"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F47"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fmcw_demo: small improvment list below
1. update pinout doc;
2. use spi4 soft cs;
3. encapsulate usb handle;
4. use o2 project optimise option.
</commit_message>
<xml_diff>
--- a/embeded/fmcw_demo/DOC/pin分配.xlsx
+++ b/embeded/fmcw_demo/DOC/pin分配.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A886F12-C100-4489-88D6-8CEFBEA8A791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32F429VE" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,14 +585,18 @@
   </si>
   <si>
     <t>CLK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>软cs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,22 +691,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -714,12 +719,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -761,7 +769,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,9 +801,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -827,6 +853,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1002,14 +1046,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.1328125" style="2" customWidth="1"/>
     <col min="2" max="3" width="13.73046875" style="2" customWidth="1"/>
@@ -1020,7 +1064,7 @@
     <col min="8" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1087,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1066,7 +1110,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1087,7 +1131,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1106,7 +1150,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1125,7 +1169,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1144,7 +1188,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1157,13 +1201,15 @@
       <c r="D7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1184,7 +1230,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1203,7 +1249,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1224,7 +1270,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1243,7 +1289,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1262,7 +1308,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1281,7 +1327,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1300,7 +1346,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1319,7 +1365,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1338,7 +1384,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1357,7 +1403,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1376,7 +1422,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1395,7 +1441,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1414,7 +1460,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1433,7 +1479,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1450,7 +1496,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1467,7 +1513,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1488,7 +1534,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1505,7 +1551,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1526,7 +1572,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1543,7 +1589,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1562,7 +1608,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1579,7 +1625,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1600,7 +1646,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1617,7 +1663,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1634,7 +1680,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1651,7 +1697,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1668,7 +1714,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1685,7 +1731,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1702,7 +1748,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1719,7 +1765,7 @@
       <c r="F37" s="5"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1736,7 +1782,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1753,7 +1799,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1770,7 +1816,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1787,7 +1833,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1804,7 +1850,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1821,7 +1867,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1838,7 +1884,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1855,7 +1901,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1872,7 +1918,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1889,7 +1935,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1908,7 +1954,7 @@
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1925,7 +1971,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
fmcw_demo: update pinout doc
</commit_message>
<xml_diff>
--- a/embeded/fmcw_demo/DOC/pin分配.xlsx
+++ b/embeded/fmcw_demo/DOC/pin分配.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A886F12-C100-4489-88D6-8CEFBEA8A791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C924559-7214-4D91-928A-E764A5D5B569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="152">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -589,6 +589,14 @@
   </si>
   <si>
     <t>软cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常低高复位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1049,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1492,9 +1500,13 @@
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -1509,9 +1521,13 @@
       <c r="D23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">

</xml_diff>